<commit_message>
Test case file only in test dir
</commit_message>
<xml_diff>
--- a/test/test_case.xlsx
+++ b/test/test_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/Library/Group Containers/G69SCX94XU.duck/Library/Application Support/duck/Volumes.noindex/DPB-DGE Data Transfer Node/nobackup/scratch/awongel/clab_pypsa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/CLab/clab_pypsa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADF4961-E8C8-3041-A0E0-08B97853B78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F836BA01-8361-8C4A-8DB6-C57AFE73745A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="500" windowWidth="27920" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="880" windowWidth="28500" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input_intermodel_one_node_" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="111">
   <si>
     <t>Note that demand has no decisions.</t>
   </si>
@@ -354,6 +354,18 @@
   </si>
   <si>
     <t>/carnegie/data/Shared/Labs/Caldeira Lab/Everyone/energy_demand_capacity_data/test_case_solar_wind_demand/</t>
+  </si>
+  <si>
+    <t>costs_path</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/PyPSA/technology-data/master/outputs/costs_2020.csv</t>
+  </si>
+  <si>
+    <t>p_min_pu</t>
+  </si>
+  <si>
+    <t>Note: p_min_pu allow bidirectionality of link</t>
   </si>
 </sst>
 </file>
@@ -363,7 +375,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -510,6 +522,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="36">
@@ -889,7 +908,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -927,6 +946,8 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1282,9 +1303,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S76"/>
+  <dimension ref="A1:T77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -1544,840 +1565,833 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" t="s">
-        <v>44</v>
+        <v>107</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" t="s">
-        <v>46</v>
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C30" s="8"/>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" s="10"/>
+        <v>43</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="8"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="10"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>99</v>
       </c>
-      <c r="B32" s="21">
-        <f>(B30-B29)*24/B31</f>
+      <c r="B33" s="21">
+        <f>(B31-B30)*24/B32</f>
         <v>8784</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>100</v>
       </c>
-      <c r="B33" s="21">
-        <f>B32*B31</f>
+      <c r="B34" s="21">
+        <f>B33*B32</f>
         <v>8784</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B36" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" t="s">
+      <c r="C36" s="7"/>
+      <c r="D36" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B37" s="1">
         <v>10000000000</v>
       </c>
-      <c r="C36" s="1"/>
-      <c r="D36" t="s">
+      <c r="C37" s="1"/>
+      <c r="D37" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>78</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>79</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="F42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>18</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I43" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="D43" t="s">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
         <v>76</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H44" t="s">
         <v>83</v>
       </c>
-      <c r="O43" t="s">
+      <c r="O44" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+    <row r="45" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+    <row r="46" spans="1:18" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D46" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G45" s="4" t="s">
+      <c r="H46" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H45" s="4" t="s">
+      <c r="I46" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I45" s="4" t="s">
+      <c r="J46" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K45" s="4" t="s">
+      <c r="L46" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M45" s="4" t="s">
+      <c r="N46" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O45" s="5" t="s">
+      <c r="P46" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5" t="s">
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:17" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:18" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F48" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="H48" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="I48" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I47" s="2" t="s">
+      <c r="J48" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K47" s="2" t="s">
+      <c r="L48" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M47" s="2" t="s">
+      <c r="N48" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N47" s="2" t="s">
+      <c r="O48" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O47" s="2" t="s">
+      <c r="P48" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P47" s="2" t="s">
+      <c r="Q48" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="Q47" s="2" t="s">
+      <c r="R48" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>28</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>28</v>
-      </c>
-      <c r="D48" t="s">
-        <v>22</v>
-      </c>
-      <c r="F48" t="s">
-        <v>50</v>
-      </c>
-      <c r="I48" s="21">
-        <f>L68*B33</f>
-        <v>171.65443408509168</v>
-      </c>
-      <c r="J48" t="str">
-        <f>B40 &amp; "/time range/" &amp; B39</f>
-        <v>$/time range/kW</v>
-      </c>
-      <c r="K48" s="15"/>
-      <c r="L48" t="str">
-        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
-        <v>$/kWh</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B49" t="s">
-        <v>19</v>
-      </c>
-      <c r="C49" t="s">
-        <v>19</v>
       </c>
       <c r="D49" t="s">
         <v>22</v>
       </c>
-      <c r="F49" t="s">
-        <v>51</v>
-      </c>
-      <c r="I49" s="15"/>
-      <c r="K49" s="15"/>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G49" t="s">
+        <v>50</v>
+      </c>
+      <c r="J49" s="21">
+        <f>L69*B34</f>
+        <v>171.65443408509168</v>
+      </c>
+      <c r="K49" t="str">
+        <f>B41 &amp; "/time range/" &amp; B40</f>
+        <v>$/time range/kW</v>
+      </c>
+      <c r="L49" s="15"/>
+      <c r="M49" t="str">
+        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
+        <v>$/kWh</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C50" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D50" t="s">
         <v>22</v>
       </c>
-      <c r="I50" s="21">
-        <f>L69*B33</f>
-        <v>104.08824719790415</v>
-      </c>
-      <c r="J50" t="str">
-        <f>B40 &amp; "/time range/" &amp; B39</f>
-        <v>$/time range/kW</v>
-      </c>
-      <c r="K50" s="15">
-        <f>H69 + I69/J69</f>
-        <v>3.9088110924995347E-2</v>
-      </c>
-      <c r="L50" t="str">
-        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
-        <v>$/kWh</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G50" t="s">
+        <v>51</v>
+      </c>
+      <c r="J50" s="15"/>
+      <c r="L50" s="15"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D51" t="s">
         <v>22</v>
       </c>
-      <c r="I51" s="21">
-        <f>L70*M51*B33</f>
-        <v>223.87212597208145</v>
-      </c>
-      <c r="J51" t="str">
-        <f>B40 &amp; "/time range/" &amp; B39</f>
+      <c r="J51" s="21">
+        <f>L70*B34</f>
+        <v>104.08824719790415</v>
+      </c>
+      <c r="K51" t="str">
+        <f>B41 &amp; "/time range/" &amp; B40</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K51" s="15"/>
-      <c r="L51" t="str">
-        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
+      <c r="L51" s="15">
+        <f>H70 + I70/J70</f>
+        <v>3.9088110924995347E-2</v>
+      </c>
+      <c r="M51" t="str">
+        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
         <v>$/kWh</v>
       </c>
-      <c r="M51">
-        <v>6.008</v>
-      </c>
-      <c r="N51" t="b">
-        <v>1</v>
-      </c>
-      <c r="O51">
-        <v>0.9</v>
-      </c>
-      <c r="Q51">
-        <v>1.1400000000000001E-6</v>
-      </c>
-      <c r="R51" t="str">
-        <f xml:space="preserve"> 1 &amp; "/" &amp; B38</f>
-        <v>1/h</v>
-      </c>
-      <c r="S51" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B52" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C52" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D52" t="s">
         <v>22</v>
       </c>
-      <c r="I52" s="21">
-        <f>L71*B33</f>
-        <v>548.78374889246641</v>
-      </c>
-      <c r="J52" t="str">
-        <f>B40 &amp; "/time range/" &amp; B39</f>
+      <c r="J52" s="21">
+        <f>L71*N52*B34</f>
+        <v>223.87212597208145</v>
+      </c>
+      <c r="K52" t="str">
+        <f>B41 &amp; "/time range/" &amp; B40</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K52" s="15">
-        <f>H71 + I71/J71</f>
-        <v>2.5047272727272724E-2</v>
-      </c>
-      <c r="L52" t="str">
-        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
+      <c r="L52" s="15"/>
+      <c r="M52" t="str">
+        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
         <v>$/kWh</v>
       </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="N52">
+        <v>6.008</v>
+      </c>
+      <c r="O52" t="b">
+        <v>1</v>
+      </c>
+      <c r="P52">
+        <v>0.9</v>
+      </c>
+      <c r="R52">
+        <v>1.1400000000000001E-6</v>
+      </c>
+      <c r="S52" t="str">
+        <f xml:space="preserve"> 1 &amp; "/" &amp; B39</f>
+        <v>1/h</v>
+      </c>
+      <c r="T52" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D53" t="s">
         <v>22</v>
       </c>
-      <c r="F53" t="s">
-        <v>52</v>
-      </c>
-      <c r="I53" s="21">
-        <f>L72*B33</f>
-        <v>181.49756560590552</v>
-      </c>
-      <c r="J53" t="str">
-        <f>B40 &amp; "/time range/" &amp; B39</f>
+      <c r="J53" s="21">
+        <f>L72*B34</f>
+        <v>548.78374889246641</v>
+      </c>
+      <c r="K53" t="str">
+        <f>B41 &amp; "/time range/" &amp; B40</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K53" s="15"/>
-      <c r="L53" t="str">
-        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
+      <c r="L53" s="15">
+        <f>H72 + I72/J72</f>
+        <v>2.5047272727272724E-2</v>
+      </c>
+      <c r="M53" t="str">
+        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
         <v>$/kWh</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C54" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D54" t="s">
         <v>22</v>
       </c>
-      <c r="E54" t="s">
+      <c r="G54" t="s">
+        <v>52</v>
+      </c>
+      <c r="J54" s="21">
+        <f>L73*B34</f>
+        <v>181.49756560590552</v>
+      </c>
+      <c r="K54" t="str">
+        <f>B41 &amp; "/time range/" &amp; B40</f>
+        <v>$/time range/kW</v>
+      </c>
+      <c r="L54" s="15"/>
+      <c r="M54" t="str">
+        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
+        <v>$/kWh</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" t="s">
+        <v>36</v>
+      </c>
+      <c r="C55" t="s">
+        <v>36</v>
+      </c>
+      <c r="D55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E55" t="s">
         <v>38</v>
       </c>
-      <c r="I54" s="21">
-        <f>L73*B33</f>
+      <c r="J55" s="21">
+        <f>L74*B34</f>
         <v>43.92</v>
       </c>
-      <c r="J54" t="str">
-        <f>B40 &amp; "/time range/" &amp; B39</f>
+      <c r="K55" t="str">
+        <f>B41 &amp; "/time range/" &amp; B40</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K54" s="15"/>
-      <c r="L54" t="str">
-        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
+      <c r="L55" s="15"/>
+      <c r="M55" t="str">
+        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
         <v>$/kWh</v>
       </c>
-      <c r="O54">
+      <c r="P55">
         <v>0.7</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A55" s="8" t="s">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A56" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>39</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>39</v>
-      </c>
-      <c r="D55" t="s">
-        <v>38</v>
-      </c>
-      <c r="I55" s="21">
-        <f>L74*B33</f>
-        <v>0.140544</v>
-      </c>
-      <c r="J55" t="str">
-        <f>B40 &amp; "/time range/" &amp; B39 &amp; B38</f>
-        <v>$/time range/kWh</v>
-      </c>
-      <c r="K55" s="15"/>
-      <c r="L55" t="str">
-        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
-        <v>$/kWh</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A56" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B56" t="s">
-        <v>40</v>
-      </c>
-      <c r="C56" t="s">
-        <v>40</v>
       </c>
       <c r="D56" t="s">
         <v>38</v>
       </c>
-      <c r="E56" t="s">
+      <c r="J56" s="21">
+        <f>L75*B34</f>
+        <v>0.140544</v>
+      </c>
+      <c r="K56" t="str">
+        <f>B41 &amp; "/time range/" &amp; B40 &amp; B39</f>
+        <v>$/time range/kWh</v>
+      </c>
+      <c r="L56" s="15"/>
+      <c r="M56" t="str">
+        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
+        <v>$/kWh</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B57" t="s">
+        <v>40</v>
+      </c>
+      <c r="C57" t="s">
+        <v>40</v>
+      </c>
+      <c r="D57" t="s">
+        <v>38</v>
+      </c>
+      <c r="E57" t="s">
         <v>22</v>
       </c>
-      <c r="I56" s="21">
-        <f>L75*B33</f>
+      <c r="J57" s="21">
+        <f>L76*B34</f>
         <v>17.568000000000001</v>
       </c>
-      <c r="J56" t="str">
-        <f>B40 &amp; "/time range/" &amp; B39</f>
+      <c r="K57" t="str">
+        <f>B41 &amp; "/time range/" &amp; B40</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K56" s="15"/>
-      <c r="L56" t="str">
-        <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
+      <c r="L57" s="15"/>
+      <c r="M57" t="str">
+        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
         <v>$/kWh</v>
       </c>
-      <c r="O56">
+      <c r="P57">
         <v>0.5</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A62" s="15" t="s">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A63" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B62" s="15"/>
-      <c r="C62" s="15"/>
-      <c r="L62" s="9"/>
-      <c r="M62" s="9"/>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>89</v>
-      </c>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
       <c r="L63" s="9"/>
       <c r="M63" s="9"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A65" s="12" t="s">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>89</v>
+      </c>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A66" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="11"/>
-      <c r="K65" s="11"/>
-      <c r="L65" s="2"/>
-      <c r="M65" s="2"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A66" s="12"/>
-      <c r="B66" s="16" t="s">
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="11"/>
+      <c r="J66" s="11"/>
+      <c r="K66" s="11"/>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A67" s="12"/>
+      <c r="B67" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C66" s="14">
+      <c r="C67" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D66" s="16"/>
-      <c r="E66" s="16"/>
-      <c r="F66" s="16"/>
-      <c r="G66" s="16"/>
-      <c r="H66" s="16"/>
-      <c r="I66" s="16"/>
-      <c r="J66" s="16"/>
-      <c r="K66" s="16"/>
-      <c r="L66" s="16"/>
-      <c r="M66" s="16"/>
-    </row>
-    <row r="67" spans="1:13" ht="64" x14ac:dyDescent="0.2">
-      <c r="A67" s="2"/>
-      <c r="B67" s="13" t="s">
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="16"/>
+      <c r="K67" s="16"/>
+      <c r="L67" s="16"/>
+      <c r="M67" s="16"/>
+    </row>
+    <row r="68" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="A68" s="2"/>
+      <c r="B68" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C67" s="19" t="str">
-        <f xml:space="preserve"> "Overnight cost [" &amp; B40 &amp; "/" &amp; B39 &amp; "]"</f>
+      <c r="C68" s="19" t="str">
+        <f xml:space="preserve"> "Overnight cost [" &amp; B41 &amp; "/" &amp; B40 &amp; "]"</f>
         <v>Overnight cost [$/kW]</v>
       </c>
-      <c r="D67" s="13" t="str">
-        <f xml:space="preserve"> "Fixed O&amp;M cost ["  &amp; B40 &amp; "/" &amp; B39 &amp; "year]"</f>
+      <c r="D68" s="13" t="str">
+        <f xml:space="preserve"> "Fixed O&amp;M cost ["  &amp; B41 &amp; "/" &amp; B40 &amp; "year]"</f>
         <v>Fixed O&amp;M cost [$/kWyear]</v>
       </c>
-      <c r="E67" s="13" t="s">
+      <c r="E68" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F67" s="13" t="s">
+      <c r="F68" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="G67" s="17" t="str">
-        <f xml:space="preserve"> "Annual fixed costs [" &amp;B40 &amp; "/year]"</f>
+      <c r="G68" s="17" t="str">
+        <f xml:space="preserve"> "Annual fixed costs [" &amp;B41 &amp; "/year]"</f>
         <v>Annual fixed costs [$/year]</v>
       </c>
-      <c r="H67" s="13" t="str">
-        <f xml:space="preserve"> "Variable O&amp;M [" &amp; B40 &amp; "/" &amp; B39 &amp; B38 &amp; "]"</f>
+      <c r="H68" s="13" t="str">
+        <f xml:space="preserve"> "Variable O&amp;M [" &amp; B41 &amp; "/" &amp; B40 &amp; B39 &amp; "]"</f>
         <v>Variable O&amp;M [$/kWh]</v>
       </c>
-      <c r="I67" s="13" t="str">
-        <f xml:space="preserve"> "Fuel cost [" &amp; B40 &amp; "/" &amp; B39 &amp; B38 &amp; "]"</f>
+      <c r="I68" s="13" t="str">
+        <f xml:space="preserve"> "Fuel cost [" &amp; B41 &amp; "/" &amp; B40 &amp; B39 &amp; "]"</f>
         <v>Fuel cost [$/kWh]</v>
       </c>
-      <c r="J67" s="13" t="s">
+      <c r="J68" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="K67" s="19"/>
-      <c r="L67" s="13" t="s">
+      <c r="K68" s="19"/>
+      <c r="L68" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="M67" s="13"/>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B68" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C68" s="20">
-        <v>1851</v>
-      </c>
-      <c r="D68" s="14">
-        <v>22.02</v>
-      </c>
-      <c r="E68" s="14">
-        <f>C66*(1+C66)^F68/((1+C66)^F68-1)</f>
-        <v>8.0586403511111196E-2</v>
-      </c>
-      <c r="F68" s="14">
-        <v>30</v>
-      </c>
-      <c r="G68" s="18">
-        <f>C68*E68+D68</f>
-        <v>171.18543289906683</v>
-      </c>
-      <c r="H68" s="14"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="14"/>
-      <c r="K68" s="20"/>
-      <c r="L68" s="14">
-        <f>G68/8760</f>
-        <v>1.954171608436836E-2</v>
-      </c>
-      <c r="M68" s="14" t="str">
-        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
-        <v>$/h/kW</v>
-      </c>
+      <c r="M68" s="13"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B69" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C69" s="20">
-        <v>982</v>
+        <v>1851</v>
       </c>
       <c r="D69" s="14">
-        <v>11.11</v>
+        <v>22.02</v>
       </c>
       <c r="E69" s="14">
-        <f>C66*(1+C66)^F69/((1+C66)^F69-1)</f>
-        <v>9.4392925743255696E-2</v>
+        <f>C67*(1+C67)^F69/((1+C67)^F69-1)</f>
+        <v>8.0586403511111196E-2</v>
       </c>
       <c r="F69" s="14">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G69" s="18">
         <f>C69*E69+D69</f>
-        <v>103.80385307987709</v>
-      </c>
-      <c r="H69" s="14">
-        <v>3.5400000000000002E-3</v>
-      </c>
-      <c r="I69" s="14">
-        <v>1.9099999999999999E-2</v>
-      </c>
-      <c r="J69" s="14">
-        <v>0.5373</v>
-      </c>
+        <v>171.18543289906683</v>
+      </c>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
       <c r="K69" s="20"/>
       <c r="L69" s="14">
         <f>G69/8760</f>
-        <v>1.1849754917794188E-2</v>
+        <v>1.954171608436836E-2</v>
       </c>
       <c r="M69" s="14" t="str">
-        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B70" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C70" s="20">
-        <v>261</v>
-      </c>
-      <c r="D70" s="14"/>
+        <v>982</v>
+      </c>
+      <c r="D70" s="14">
+        <v>11.11</v>
+      </c>
       <c r="E70" s="14">
-        <f>C66*(1+C66)^F70/((1+C66)^F70-1)</f>
-        <v>0.14237750272736471</v>
+        <f>C67*(1+C67)^F70/((1+C67)^F70-1)</f>
+        <v>9.4392925743255696E-2</v>
       </c>
       <c r="F70" s="14">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G70" s="18">
         <f>C70*E70+D70</f>
-        <v>37.160528211842191</v>
-      </c>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="14"/>
+        <v>103.80385307987709</v>
+      </c>
+      <c r="H70" s="14">
+        <v>3.5400000000000002E-3</v>
+      </c>
+      <c r="I70" s="14">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="J70" s="14">
+        <v>0.5373</v>
+      </c>
       <c r="K70" s="20"/>
       <c r="L70" s="14">
         <f>G70/8760</f>
-        <v>4.2420694305755928E-3</v>
+        <v>1.1849754917794188E-2</v>
       </c>
       <c r="M70" s="14" t="str">
-        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B71" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C71" s="20">
-        <v>5946</v>
-      </c>
-      <c r="D71" s="14">
-        <v>101.28</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="D71" s="14"/>
       <c r="E71" s="14">
-        <f>C66*(1+C66)^F71/((1+C66)^F71-1)</f>
-        <v>7.5009138873610326E-2</v>
+        <f>C67*(1+C67)^F71/((1+C67)^F71-1)</f>
+        <v>0.14237750272736471</v>
       </c>
       <c r="F71" s="14">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G71" s="18">
         <f>C71*E71+D71</f>
-        <v>547.28433974248696</v>
-      </c>
-      <c r="H71" s="14">
-        <v>2.32E-3</v>
-      </c>
-      <c r="I71" s="14">
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="J71" s="14">
-        <v>0.33</v>
-      </c>
+        <v>37.160528211842191</v>
+      </c>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
       <c r="K71" s="20"/>
       <c r="L71" s="14">
         <f>G71/8760</f>
-        <v>6.2475381249142349E-2</v>
+        <v>4.2420694305755928E-3</v>
       </c>
       <c r="M71" s="14" t="str">
-        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B72" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C72" s="20">
-        <v>1657</v>
+        <v>5946</v>
       </c>
       <c r="D72" s="14">
-        <v>47.47</v>
+        <v>101.28</v>
       </c>
       <c r="E72" s="14">
-        <f>C66*(1+C66)^F72/((1+C66)^F72-1)</f>
-        <v>8.0586403511111196E-2</v>
+        <f>C67*(1+C67)^F72/((1+C67)^F72-1)</f>
+        <v>7.5009138873610326E-2</v>
       </c>
       <c r="F72" s="14">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G72" s="18">
         <f>C72*E72+D72</f>
-        <v>181.00167061791126</v>
-      </c>
-      <c r="H72" s="14"/>
-      <c r="I72" s="14"/>
-      <c r="J72" s="14"/>
+        <v>547.28433974248696</v>
+      </c>
+      <c r="H72" s="14">
+        <v>2.32E-3</v>
+      </c>
+      <c r="I72" s="14">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="J72" s="14">
+        <v>0.33</v>
+      </c>
       <c r="K72" s="20"/>
       <c r="L72" s="14">
         <f>G72/8760</f>
-        <v>2.0662291166428225E-2</v>
+        <v>6.2475381249142349E-2</v>
       </c>
       <c r="M72" s="14" t="str">
-        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B73" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C73" s="20"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="18"/>
+        <v>34</v>
+      </c>
+      <c r="C73" s="20">
+        <v>1657</v>
+      </c>
+      <c r="D73" s="14">
+        <v>47.47</v>
+      </c>
+      <c r="E73" s="14">
+        <f>C67*(1+C67)^F73/((1+C67)^F73-1)</f>
+        <v>8.0586403511111196E-2</v>
+      </c>
+      <c r="F73" s="14">
+        <v>30</v>
+      </c>
+      <c r="G73" s="18">
+        <f>C73*E73+D73</f>
+        <v>181.00167061791126</v>
+      </c>
       <c r="H73" s="14"/>
       <c r="I73" s="14"/>
-      <c r="J73" s="18"/>
-      <c r="K73" s="14"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="20"/>
       <c r="L73" s="14">
-        <v>5.0000000000000001E-3</v>
+        <f>G73/8760</f>
+        <v>2.0662291166428225E-2</v>
       </c>
       <c r="M73" s="14" t="str">
-        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B74" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C74" s="20"/>
       <c r="D74" s="14"/>
@@ -2389,16 +2403,16 @@
       <c r="J74" s="18"/>
       <c r="K74" s="14"/>
       <c r="L74" s="14">
-        <v>1.5999999999999999E-5</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="M74" s="14" t="str">
-        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B75" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C75" s="20"/>
       <c r="D75" s="14"/>
@@ -2410,15 +2424,36 @@
       <c r="J75" s="18"/>
       <c r="K75" s="14"/>
       <c r="L75" s="14">
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="M75" s="14" t="str">
+        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
+        <v>$/h/kW</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B76" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C76" s="20"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="14"/>
+      <c r="I76" s="14"/>
+      <c r="J76" s="18"/>
+      <c r="K76" s="14"/>
+      <c r="L76" s="14">
         <v>2E-3</v>
       </c>
-      <c r="M75" s="14" t="str">
-        <f>B40&amp;"/"&amp;B38&amp;"/"&amp;B39</f>
+      <c r="M76" s="14" t="str">
+        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
         <v>$/h/kW</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B76" t="s">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
scaling revisited and venv
</commit_message>
<xml_diff>
--- a/test/test_case.xlsx
+++ b/test/test_case.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/CLab/clab_pypsa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/CLab/clab_pypsa/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F836BA01-8361-8C4A-8DB6-C57AFE73745A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1353A4C-BE3C-9547-A6BB-C12A1AD566B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="880" windowWidth="28500" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="113">
   <si>
     <t>Note that demand has no decisions.</t>
   </si>
@@ -366,6 +366,12 @@
   </si>
   <si>
     <t>Note: p_min_pu allow bidirectionality of link</t>
+  </si>
+  <si>
+    <t>solver</t>
+  </si>
+  <si>
+    <t>gurobi</t>
   </si>
 </sst>
 </file>
@@ -947,7 +953,9 @@
     <xf numFmtId="49" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1303,10 +1311,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T77"/>
+  <dimension ref="A1:T78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1652,331 +1660,310 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" t="s">
-        <v>59</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" s="6"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B38" s="1">
         <v>10000000000</v>
       </c>
-      <c r="C37" s="1"/>
-      <c r="D37" t="s">
+      <c r="C38" s="1"/>
+      <c r="D38" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-    </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>77</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="F42" t="s">
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="F43" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>18</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I44" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D44" t="s">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
         <v>76</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H45" t="s">
         <v>83</v>
       </c>
-      <c r="O44" t="s">
+      <c r="O45" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+    <row r="46" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:18" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+    <row r="47" spans="1:18" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D47" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H46" s="4" t="s">
+      <c r="H47" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I46" s="4" t="s">
+      <c r="I47" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J46" s="4" t="s">
+      <c r="J47" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L46" s="4" t="s">
+      <c r="L47" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N46" s="4" t="s">
+      <c r="N47" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="P46" s="5" t="s">
+      <c r="P47" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5" t="s">
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="1:18" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+    <row r="49" spans="1:20" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F48" s="24" t="s">
+      <c r="F49" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I48" s="2" t="s">
+      <c r="I49" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J48" s="2" t="s">
+      <c r="J49" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L48" s="2" t="s">
+      <c r="L49" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N48" s="2" t="s">
+      <c r="N49" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O48" s="2" t="s">
+      <c r="O49" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P48" s="2" t="s">
+      <c r="P49" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q48" s="2" t="s">
+      <c r="Q49" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="R48" s="2" t="s">
+      <c r="R49" s="2" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" t="s">
-        <v>28</v>
-      </c>
-      <c r="C49" t="s">
-        <v>28</v>
-      </c>
-      <c r="D49" t="s">
-        <v>22</v>
-      </c>
-      <c r="G49" t="s">
-        <v>50</v>
-      </c>
-      <c r="J49" s="21">
-        <f>L69*B34</f>
-        <v>171.65443408509168</v>
-      </c>
-      <c r="K49" t="str">
-        <f>B41 &amp; "/time range/" &amp; B40</f>
-        <v>$/time range/kW</v>
-      </c>
-      <c r="L49" s="15"/>
-      <c r="M49" t="str">
-        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
-        <v>$/kWh</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B50" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C50" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D50" t="s">
         <v>22</v>
       </c>
       <c r="G50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J50" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="J50" s="21">
+        <f>L70*B34</f>
+        <v>171.65443408509168</v>
+      </c>
+      <c r="K50" t="str">
+        <f>B42 &amp; "/time range/" &amp; B41</f>
+        <v>$/time range/kW</v>
+      </c>
       <c r="L50" s="15"/>
+      <c r="M50" t="str">
+        <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
+        <v>$/kWh</v>
+      </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C51" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D51" t="s">
         <v>22</v>
       </c>
-      <c r="J51" s="21">
-        <f>L70*B34</f>
-        <v>104.08824719790415</v>
-      </c>
-      <c r="K51" t="str">
-        <f>B41 &amp; "/time range/" &amp; B40</f>
-        <v>$/time range/kW</v>
-      </c>
-      <c r="L51" s="15">
-        <f>H70 + I70/J70</f>
-        <v>3.9088110924995347E-2</v>
-      </c>
-      <c r="M51" t="str">
-        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
-        <v>$/kWh</v>
-      </c>
+      <c r="G51" t="s">
+        <v>51</v>
+      </c>
+      <c r="J51" s="15"/>
+      <c r="L51" s="15"/>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C52" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D52" t="s">
         <v>22</v>
       </c>
       <c r="J52" s="21">
-        <f>L71*N52*B34</f>
-        <v>223.87212597208145</v>
+        <f>L71*B34</f>
+        <v>104.08824719790415</v>
       </c>
       <c r="K52" t="str">
-        <f>B41 &amp; "/time range/" &amp; B40</f>
+        <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L52" s="15"/>
+      <c r="L52" s="15">
+        <f>H71 + I71/J71</f>
+        <v>3.9088110924995347E-2</v>
+      </c>
       <c r="M52" t="str">
-        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
+        <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
-      </c>
-      <c r="N52">
-        <v>6.008</v>
-      </c>
-      <c r="O52" t="b">
-        <v>1</v>
-      </c>
-      <c r="P52">
-        <v>0.9</v>
-      </c>
-      <c r="R52">
-        <v>1.1400000000000001E-6</v>
-      </c>
-      <c r="S52" t="str">
-        <f xml:space="preserve"> 1 &amp; "/" &amp; B39</f>
-        <v>1/h</v>
-      </c>
-      <c r="T52" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C53" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D53" t="s">
         <v>22</v>
       </c>
       <c r="J53" s="21">
-        <f>L72*B34</f>
-        <v>548.78374889246641</v>
+        <f>L72*N53*B34</f>
+        <v>223.87212597208145</v>
       </c>
       <c r="K53" t="str">
-        <f>B41 &amp; "/time range/" &amp; B40</f>
+        <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L53" s="15">
-        <f>H72 + I72/J72</f>
-        <v>2.5047272727272724E-2</v>
-      </c>
+      <c r="L53" s="15"/>
       <c r="M53" t="str">
-        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
+        <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
+      </c>
+      <c r="N53">
+        <v>6.008</v>
+      </c>
+      <c r="O53" t="b">
+        <v>1</v>
+      </c>
+      <c r="P53">
+        <v>0.9</v>
+      </c>
+      <c r="R53">
+        <v>1.1400000000000001E-6</v>
+      </c>
+      <c r="S53" t="str">
+        <f xml:space="preserve"> 1 &amp; "/" &amp; B40</f>
+        <v>1/h</v>
+      </c>
+      <c r="T53" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
@@ -1984,435 +1971,444 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C54" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D54" t="s">
         <v>22</v>
       </c>
-      <c r="G54" t="s">
-        <v>52</v>
-      </c>
       <c r="J54" s="21">
         <f>L73*B34</f>
-        <v>181.49756560590552</v>
+        <v>548.78374889246641</v>
       </c>
       <c r="K54" t="str">
-        <f>B41 &amp; "/time range/" &amp; B40</f>
+        <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L54" s="15"/>
+      <c r="L54" s="15">
+        <f>H73 + I73/J73</f>
+        <v>2.5047272727272724E-2</v>
+      </c>
       <c r="M54" t="str">
-        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
+        <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C55" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D55" t="s">
         <v>22</v>
       </c>
-      <c r="E55" t="s">
-        <v>38</v>
+      <c r="G55" t="s">
+        <v>52</v>
       </c>
       <c r="J55" s="21">
         <f>L74*B34</f>
-        <v>43.92</v>
+        <v>181.49756560590552</v>
       </c>
       <c r="K55" t="str">
-        <f>B41 &amp; "/time range/" &amp; B40</f>
+        <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
       <c r="L55" s="15"/>
       <c r="M55" t="str">
-        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
+        <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
-      </c>
-      <c r="P55">
-        <v>0.7</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B56" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C56" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D56" t="s">
+        <v>22</v>
+      </c>
+      <c r="E56" t="s">
         <v>38</v>
       </c>
       <c r="J56" s="21">
         <f>L75*B34</f>
-        <v>0.140544</v>
+        <v>43.92</v>
       </c>
       <c r="K56" t="str">
-        <f>B41 &amp; "/time range/" &amp; B40 &amp; B39</f>
-        <v>$/time range/kWh</v>
+        <f>B42 &amp; "/time range/" &amp; B41</f>
+        <v>$/time range/kW</v>
       </c>
       <c r="L56" s="15"/>
       <c r="M56" t="str">
-        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
+        <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
+      </c>
+      <c r="P56">
+        <v>0.7</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B57" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C57" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D57" t="s">
         <v>38</v>
       </c>
-      <c r="E57" t="s">
-        <v>22</v>
-      </c>
       <c r="J57" s="21">
         <f>L76*B34</f>
-        <v>17.568000000000001</v>
+        <v>0.140544</v>
       </c>
       <c r="K57" t="str">
-        <f>B41 &amp; "/time range/" &amp; B40</f>
-        <v>$/time range/kW</v>
+        <f>B42 &amp; "/time range/" &amp; B41 &amp; B40</f>
+        <v>$/time range/kWh</v>
       </c>
       <c r="L57" s="15"/>
       <c r="M57" t="str">
-        <f xml:space="preserve"> B41 &amp; "/" &amp; B40 &amp; B39</f>
+        <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
       </c>
-      <c r="P57">
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A58" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" t="s">
+        <v>40</v>
+      </c>
+      <c r="C58" t="s">
+        <v>40</v>
+      </c>
+      <c r="D58" t="s">
+        <v>38</v>
+      </c>
+      <c r="E58" t="s">
+        <v>22</v>
+      </c>
+      <c r="J58" s="21">
+        <f>L77*B34</f>
+        <v>17.568000000000001</v>
+      </c>
+      <c r="K58" t="str">
+        <f>B42 &amp; "/time range/" &amp; B41</f>
+        <v>$/time range/kW</v>
+      </c>
+      <c r="L58" s="15"/>
+      <c r="M58" t="str">
+        <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
+        <v>$/kWh</v>
+      </c>
+      <c r="P58">
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A63" s="15" t="s">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A64" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B63" s="15"/>
-      <c r="C63" s="15"/>
-      <c r="L63" s="9"/>
-      <c r="M63" s="9"/>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>89</v>
-      </c>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
       <c r="L64" s="9"/>
       <c r="M64" s="9"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A66" s="12" t="s">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>89</v>
+      </c>
+      <c r="L65" s="9"/>
+      <c r="M65" s="9"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A67" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-      <c r="I66" s="11"/>
-      <c r="J66" s="11"/>
-      <c r="K66" s="11"/>
-      <c r="L66" s="2"/>
-      <c r="M66" s="2"/>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A67" s="12"/>
-      <c r="B67" s="16" t="s">
+      <c r="B67" s="11"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="11"/>
+      <c r="J67" s="11"/>
+      <c r="K67" s="11"/>
+      <c r="L67" s="2"/>
+      <c r="M67" s="2"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A68" s="12"/>
+      <c r="B68" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C67" s="14">
+      <c r="C68" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D67" s="16"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
-      <c r="G67" s="16"/>
-      <c r="H67" s="16"/>
-      <c r="I67" s="16"/>
-      <c r="J67" s="16"/>
-      <c r="K67" s="16"/>
-      <c r="L67" s="16"/>
-      <c r="M67" s="16"/>
-    </row>
-    <row r="68" spans="1:13" ht="64" x14ac:dyDescent="0.2">
-      <c r="A68" s="2"/>
-      <c r="B68" s="13" t="s">
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="16"/>
+      <c r="I68" s="16"/>
+      <c r="J68" s="16"/>
+      <c r="K68" s="16"/>
+      <c r="L68" s="16"/>
+      <c r="M68" s="16"/>
+    </row>
+    <row r="69" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="A69" s="2"/>
+      <c r="B69" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C68" s="19" t="str">
-        <f xml:space="preserve"> "Overnight cost [" &amp; B41 &amp; "/" &amp; B40 &amp; "]"</f>
+      <c r="C69" s="19" t="str">
+        <f xml:space="preserve"> "Overnight cost [" &amp; B42 &amp; "/" &amp; B41 &amp; "]"</f>
         <v>Overnight cost [$/kW]</v>
       </c>
-      <c r="D68" s="13" t="str">
-        <f xml:space="preserve"> "Fixed O&amp;M cost ["  &amp; B41 &amp; "/" &amp; B40 &amp; "year]"</f>
+      <c r="D69" s="13" t="str">
+        <f xml:space="preserve"> "Fixed O&amp;M cost ["  &amp; B42 &amp; "/" &amp; B41 &amp; "year]"</f>
         <v>Fixed O&amp;M cost [$/kWyear]</v>
       </c>
-      <c r="E68" s="13" t="s">
+      <c r="E69" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F68" s="13" t="s">
+      <c r="F69" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="G68" s="17" t="str">
-        <f xml:space="preserve"> "Annual fixed costs [" &amp;B41 &amp; "/year]"</f>
+      <c r="G69" s="17" t="str">
+        <f xml:space="preserve"> "Annual fixed costs [" &amp;B42 &amp; "/year]"</f>
         <v>Annual fixed costs [$/year]</v>
       </c>
-      <c r="H68" s="13" t="str">
-        <f xml:space="preserve"> "Variable O&amp;M [" &amp; B41 &amp; "/" &amp; B40 &amp; B39 &amp; "]"</f>
+      <c r="H69" s="13" t="str">
+        <f xml:space="preserve"> "Variable O&amp;M [" &amp; B42 &amp; "/" &amp; B41 &amp; B40 &amp; "]"</f>
         <v>Variable O&amp;M [$/kWh]</v>
       </c>
-      <c r="I68" s="13" t="str">
-        <f xml:space="preserve"> "Fuel cost [" &amp; B41 &amp; "/" &amp; B40 &amp; B39 &amp; "]"</f>
+      <c r="I69" s="13" t="str">
+        <f xml:space="preserve"> "Fuel cost [" &amp; B42 &amp; "/" &amp; B41 &amp; B40 &amp; "]"</f>
         <v>Fuel cost [$/kWh]</v>
       </c>
-      <c r="J68" s="13" t="s">
+      <c r="J69" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="K68" s="19"/>
-      <c r="L68" s="13" t="s">
+      <c r="K69" s="19"/>
+      <c r="L69" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="M68" s="13"/>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B69" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C69" s="20">
-        <v>1851</v>
-      </c>
-      <c r="D69" s="14">
-        <v>22.02</v>
-      </c>
-      <c r="E69" s="14">
-        <f>C67*(1+C67)^F69/((1+C67)^F69-1)</f>
-        <v>8.0586403511111196E-2</v>
-      </c>
-      <c r="F69" s="14">
-        <v>30</v>
-      </c>
-      <c r="G69" s="18">
-        <f>C69*E69+D69</f>
-        <v>171.18543289906683</v>
-      </c>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="14"/>
-      <c r="K69" s="20"/>
-      <c r="L69" s="14">
-        <f>G69/8760</f>
-        <v>1.954171608436836E-2</v>
-      </c>
-      <c r="M69" s="14" t="str">
-        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
-        <v>$/h/kW</v>
-      </c>
+      <c r="M69" s="13"/>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B70" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C70" s="20">
-        <v>982</v>
+        <v>1851</v>
       </c>
       <c r="D70" s="14">
-        <v>11.11</v>
+        <v>22.02</v>
       </c>
       <c r="E70" s="14">
-        <f>C67*(1+C67)^F70/((1+C67)^F70-1)</f>
-        <v>9.4392925743255696E-2</v>
+        <f>C68*(1+C68)^F70/((1+C68)^F70-1)</f>
+        <v>8.0586403511111196E-2</v>
       </c>
       <c r="F70" s="14">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G70" s="18">
         <f>C70*E70+D70</f>
-        <v>103.80385307987709</v>
-      </c>
-      <c r="H70" s="14">
-        <v>3.5400000000000002E-3</v>
-      </c>
-      <c r="I70" s="14">
-        <v>1.9099999999999999E-2</v>
-      </c>
-      <c r="J70" s="14">
-        <v>0.5373</v>
-      </c>
+        <v>171.18543289906683</v>
+      </c>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="14"/>
       <c r="K70" s="20"/>
       <c r="L70" s="14">
         <f>G70/8760</f>
-        <v>1.1849754917794188E-2</v>
+        <v>1.954171608436836E-2</v>
       </c>
       <c r="M70" s="14" t="str">
-        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
+        <f>B42&amp;"/"&amp;B40&amp;"/"&amp;B41</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B71" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C71" s="20">
-        <v>261</v>
-      </c>
-      <c r="D71" s="14"/>
+        <v>982</v>
+      </c>
+      <c r="D71" s="14">
+        <v>11.11</v>
+      </c>
       <c r="E71" s="14">
-        <f>C67*(1+C67)^F71/((1+C67)^F71-1)</f>
-        <v>0.14237750272736471</v>
+        <f>C68*(1+C68)^F71/((1+C68)^F71-1)</f>
+        <v>9.4392925743255696E-2</v>
       </c>
       <c r="F71" s="14">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G71" s="18">
         <f>C71*E71+D71</f>
-        <v>37.160528211842191</v>
-      </c>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="14"/>
+        <v>103.80385307987709</v>
+      </c>
+      <c r="H71" s="14">
+        <v>3.5400000000000002E-3</v>
+      </c>
+      <c r="I71" s="14">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="J71" s="14">
+        <v>0.5373</v>
+      </c>
       <c r="K71" s="20"/>
       <c r="L71" s="14">
         <f>G71/8760</f>
-        <v>4.2420694305755928E-3</v>
+        <v>1.1849754917794188E-2</v>
       </c>
       <c r="M71" s="14" t="str">
-        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
+        <f>B42&amp;"/"&amp;B40&amp;"/"&amp;B41</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B72" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C72" s="20">
-        <v>5946</v>
-      </c>
-      <c r="D72" s="14">
-        <v>101.28</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="D72" s="14"/>
       <c r="E72" s="14">
-        <f>C67*(1+C67)^F72/((1+C67)^F72-1)</f>
-        <v>7.5009138873610326E-2</v>
+        <f>C68*(1+C68)^F72/((1+C68)^F72-1)</f>
+        <v>0.14237750272736471</v>
       </c>
       <c r="F72" s="14">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G72" s="18">
         <f>C72*E72+D72</f>
-        <v>547.28433974248696</v>
-      </c>
-      <c r="H72" s="14">
-        <v>2.32E-3</v>
-      </c>
-      <c r="I72" s="14">
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="J72" s="14">
-        <v>0.33</v>
-      </c>
+        <v>37.160528211842191</v>
+      </c>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
       <c r="K72" s="20"/>
       <c r="L72" s="14">
         <f>G72/8760</f>
-        <v>6.2475381249142349E-2</v>
+        <v>4.2420694305755928E-3</v>
       </c>
       <c r="M72" s="14" t="str">
-        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
+        <f>B42&amp;"/"&amp;B40&amp;"/"&amp;B41</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B73" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C73" s="20">
-        <v>1657</v>
+        <v>5946</v>
       </c>
       <c r="D73" s="14">
-        <v>47.47</v>
+        <v>101.28</v>
       </c>
       <c r="E73" s="14">
-        <f>C67*(1+C67)^F73/((1+C67)^F73-1)</f>
-        <v>8.0586403511111196E-2</v>
+        <f>C68*(1+C68)^F73/((1+C68)^F73-1)</f>
+        <v>7.5009138873610326E-2</v>
       </c>
       <c r="F73" s="14">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G73" s="18">
         <f>C73*E73+D73</f>
-        <v>181.00167061791126</v>
-      </c>
-      <c r="H73" s="14"/>
-      <c r="I73" s="14"/>
-      <c r="J73" s="14"/>
+        <v>547.28433974248696</v>
+      </c>
+      <c r="H73" s="14">
+        <v>2.32E-3</v>
+      </c>
+      <c r="I73" s="14">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="J73" s="14">
+        <v>0.33</v>
+      </c>
       <c r="K73" s="20"/>
       <c r="L73" s="14">
         <f>G73/8760</f>
-        <v>2.0662291166428225E-2</v>
+        <v>6.2475381249142349E-2</v>
       </c>
       <c r="M73" s="14" t="str">
-        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
+        <f>B42&amp;"/"&amp;B40&amp;"/"&amp;B41</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B74" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C74" s="20"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="18"/>
+        <v>34</v>
+      </c>
+      <c r="C74" s="20">
+        <v>1657</v>
+      </c>
+      <c r="D74" s="14">
+        <v>47.47</v>
+      </c>
+      <c r="E74" s="14">
+        <f>C68*(1+C68)^F74/((1+C68)^F74-1)</f>
+        <v>8.0586403511111196E-2</v>
+      </c>
+      <c r="F74" s="14">
+        <v>30</v>
+      </c>
+      <c r="G74" s="18">
+        <f>C74*E74+D74</f>
+        <v>181.00167061791126</v>
+      </c>
       <c r="H74" s="14"/>
       <c r="I74" s="14"/>
-      <c r="J74" s="18"/>
-      <c r="K74" s="14"/>
+      <c r="J74" s="14"/>
+      <c r="K74" s="20"/>
       <c r="L74" s="14">
-        <v>5.0000000000000001E-3</v>
+        <f>G74/8760</f>
+        <v>2.0662291166428225E-2</v>
       </c>
       <c r="M74" s="14" t="str">
-        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
+        <f>B42&amp;"/"&amp;B40&amp;"/"&amp;B41</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B75" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C75" s="20"/>
       <c r="D75" s="14"/>
@@ -2424,16 +2420,16 @@
       <c r="J75" s="18"/>
       <c r="K75" s="14"/>
       <c r="L75" s="14">
-        <v>1.5999999999999999E-5</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="M75" s="14" t="str">
-        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
+        <f>B42&amp;"/"&amp;B40&amp;"/"&amp;B41</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B76" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C76" s="20"/>
       <c r="D76" s="14"/>
@@ -2445,15 +2441,36 @@
       <c r="J76" s="18"/>
       <c r="K76" s="14"/>
       <c r="L76" s="14">
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="M76" s="14" t="str">
+        <f>B42&amp;"/"&amp;B40&amp;"/"&amp;B41</f>
+        <v>$/h/kW</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B77" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C77" s="20"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="18"/>
+      <c r="K77" s="14"/>
+      <c r="L77" s="14">
         <v>2E-3</v>
       </c>
-      <c r="M76" s="14" t="str">
-        <f>B41&amp;"/"&amp;B39&amp;"/"&amp;B40</f>
+      <c r="M77" s="14" t="str">
+        <f>B42&amp;"/"&amp;B40&amp;"/"&amp;B41</f>
         <v>$/h/kW</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B77" t="s">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test case without scaling
</commit_message>
<xml_diff>
--- a/test/test_case.xlsx
+++ b/test/test_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/CLab/clab_pypsa/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1353A4C-BE3C-9547-A6BB-C12A1AD566B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6FFBD5-D89B-7E47-B28F-A15A1ACEDA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="880" windowWidth="28500" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1314,7 +1314,7 @@
   <dimension ref="A1:T78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1684,7 +1684,7 @@
         <v>14</v>
       </c>
       <c r="B38" s="1">
-        <v>10000000000</v>
+        <v>1</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" t="s">

</xml_diff>

<commit_message>
Make solution unique for test case
</commit_message>
<xml_diff>
--- a/test/test_case.xlsx
+++ b/test/test_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/CLab/clab_pypsa/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6FFBD5-D89B-7E47-B28F-A15A1ACEDA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7FB169-7E05-FD4E-B6DB-3ADEC5362934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="880" windowWidth="28500" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1313,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1684,7 +1684,7 @@
         <v>14</v>
       </c>
       <c r="B38" s="1">
-        <v>1</v>
+        <v>10000000000</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" t="s">
@@ -1941,7 +1941,9 @@
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L53" s="15"/>
+      <c r="L53" s="15">
+        <v>0.01</v>
+      </c>
       <c r="M53" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
@@ -2050,7 +2052,9 @@
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L56" s="15"/>
+      <c r="L56" s="15">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="M56" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
@@ -2084,6 +2088,9 @@
       <c r="M57" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
+      </c>
+      <c r="R57" s="1">
+        <v>3.9999999999999998E-6</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
power unit -> power_unit
</commit_message>
<xml_diff>
--- a/test/test_case.xlsx
+++ b/test/test_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/CLab/clab_pypsa/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7FB169-7E05-FD4E-B6DB-3ADEC5362934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B12578-796C-2243-8753-7C9B1C548ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="880" windowWidth="28500" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -269,9 +269,6 @@
     <t>time_unit</t>
   </si>
   <si>
-    <t>power unit</t>
-  </si>
-  <si>
     <t>currency</t>
   </si>
   <si>
@@ -372,6 +369,9 @@
   </si>
   <si>
     <t>gurobi</t>
+  </si>
+  <si>
+    <t>power_unit</t>
   </si>
 </sst>
 </file>
@@ -1313,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1356,7 +1356,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1568,15 +1568,15 @@
         <v>45</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="23" t="s">
         <v>107</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1592,7 +1592,7 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1600,7 +1600,7 @@
         <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1608,7 +1608,7 @@
         <v>42</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" t="s">
@@ -1620,13 +1620,13 @@
         <v>43</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C31" s="8"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1635,19 +1635,19 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B33" s="21">
         <f>(B31-B30)*24/B32</f>
         <v>8784</v>
       </c>
       <c r="C33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B34" s="21">
         <f>B33*B32</f>
@@ -1660,10 +1660,10 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="24" t="s">
         <v>111</v>
-      </c>
-      <c r="B36" s="24" t="s">
-        <v>112</v>
       </c>
       <c r="C36" s="6"/>
     </row>
@@ -1700,25 +1700,25 @@
         <v>77</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C42" s="1"/>
     </row>
@@ -1726,7 +1726,7 @@
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="F43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
@@ -1734,7 +1734,7 @@
         <v>18</v>
       </c>
       <c r="I44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
@@ -1742,7 +1742,7 @@
         <v>76</v>
       </c>
       <c r="H45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O45" t="s">
         <v>75</v>
@@ -1750,7 +1750,7 @@
     </row>
     <row r="46" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:18" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -1788,7 +1788,7 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:20" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
@@ -1808,7 +1808,7 @@
         <v>37</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>53</v>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B56" t="s">
         <v>36</v>
@@ -2065,7 +2065,7 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B57" t="s">
         <v>39</v>
@@ -2095,7 +2095,7 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B58" t="s">
         <v>40</v>
@@ -2128,7 +2128,7 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
@@ -2152,14 +2152,14 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L65" s="9"/>
       <c r="M65" s="9"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B67" s="11"/>
       <c r="C67" s="11"/>
@@ -2177,7 +2177,7 @@
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="12"/>
       <c r="B68" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C68" s="14">
         <v>7.0000000000000007E-2</v>
@@ -2207,10 +2207,10 @@
         <v>Fixed O&amp;M cost [$/kWyear]</v>
       </c>
       <c r="E69" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F69" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G69" s="17" t="str">
         <f xml:space="preserve"> "Annual fixed costs [" &amp;B42 &amp; "/year]"</f>
@@ -2225,7 +2225,7 @@
         <v>Fuel cost [$/kWh]</v>
       </c>
       <c r="J69" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K69" s="19"/>
       <c r="L69" s="13" t="s">
@@ -2478,7 +2478,7 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up test_case, more Readme
</commit_message>
<xml_diff>
--- a/test/test_case.xlsx
+++ b/test/test_case.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/CLab/clab_pypsa/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B12578-796C-2243-8753-7C9B1C548ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8C1AF6-34A8-D047-B7E1-6391DB489272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="880" windowWidth="28500" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="104">
   <si>
     <t>Note that demand has no decisions.</t>
   </si>
@@ -44,30 +44,9 @@
     <t>REQUIRED KEYWORDS</t>
   </si>
   <si>
-    <t>tech_name</t>
-  </si>
-  <si>
-    <t>tech_type</t>
-  </si>
-  <si>
     <t>OPTIONAL KEYWORDS</t>
   </si>
   <si>
-    <t>node</t>
-  </si>
-  <si>
-    <t>fixed_cost</t>
-  </si>
-  <si>
-    <t>var_cost</t>
-  </si>
-  <si>
-    <t>charging_time</t>
-  </si>
-  <si>
-    <t>decay_rate</t>
-  </si>
-  <si>
     <t>CASE_DATA</t>
   </si>
   <si>
@@ -83,9 +62,6 @@
     <t>normalization</t>
   </si>
   <si>
-    <t>capacity</t>
-  </si>
-  <si>
     <t>efficiency</t>
   </si>
   <si>
@@ -302,9 +278,6 @@
     <t>Note: If there is a # in front of component (e.g. #Generator), this row will be ignored</t>
   </si>
   <si>
-    <t>MEM vocabulary</t>
-  </si>
-  <si>
     <t>delta_t</t>
   </si>
   <si>
@@ -350,9 +323,6 @@
     <t>test_case</t>
   </si>
   <si>
-    <t>/carnegie/data/Shared/Labs/Caldeira Lab/Everyone/energy_demand_capacity_data/test_case_solar_wind_demand/</t>
-  </si>
-  <si>
     <t>costs_path</t>
   </si>
   <si>
@@ -372,6 +342,9 @@
   </si>
   <si>
     <t>power_unit</t>
+  </si>
+  <si>
+    <t>test/</t>
   </si>
 </sst>
 </file>
@@ -914,17 +887,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1313,8 +1282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1338,7 +1307,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1356,7 +1325,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1394,7 +1363,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1422,10 +1391,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1434,10 +1403,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1446,10 +1415,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1466,7 +1435,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1476,10 +1445,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1488,10 +1457,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1500,10 +1469,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1512,10 +1481,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1524,10 +1493,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1536,10 +1505,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1548,10 +1517,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1560,304 +1529,266 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>105</v>
+        <v>37</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>106</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>107</v>
+        <v>96</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C30" s="8"/>
+        <v>34</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="6"/>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="6"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
-      <c r="C32" s="10"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>98</v>
-      </c>
-      <c r="B33" s="21">
+        <v>89</v>
+      </c>
+      <c r="B33" s="19">
         <f>(B31-B30)*24/B32</f>
         <v>8784</v>
       </c>
       <c r="C33" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>99</v>
-      </c>
-      <c r="B34" s="21">
+        <v>90</v>
+      </c>
+      <c r="B34" s="19">
         <f>B33*B32</f>
         <v>8784</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>110</v>
-      </c>
-      <c r="B36" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="C36" s="6"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>48</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="5"/>
       <c r="D37" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B38" s="1">
-        <v>10000000000</v>
+        <v>1</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="F43" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="I44" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D45" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H45" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="O45" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L47" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="N47" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="P47" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:20" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R49" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" t="s">
         <v>20</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N49" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O49" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P49" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q49" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="R49" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A50" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B50" t="s">
-        <v>28</v>
-      </c>
       <c r="C50" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D50" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G50" t="s">
-        <v>50</v>
-      </c>
-      <c r="J50" s="21">
+        <v>42</v>
+      </c>
+      <c r="J50" s="19">
         <f>L70*B34</f>
         <v>171.65443408509168</v>
       </c>
@@ -1865,45 +1796,45 @@
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L50" s="15"/>
+      <c r="L50" s="13"/>
       <c r="M50" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
-        <v>56</v>
+      <c r="A51" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C51" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D51" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G51" t="s">
-        <v>51</v>
-      </c>
-      <c r="J51" s="15"/>
-      <c r="L51" s="15"/>
+        <v>43</v>
+      </c>
+      <c r="J51" s="13"/>
+      <c r="L51" s="13"/>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A52" s="8" t="s">
-        <v>55</v>
+      <c r="A52" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="B52" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C52" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D52" t="s">
-        <v>22</v>
-      </c>
-      <c r="J52" s="21">
+        <v>14</v>
+      </c>
+      <c r="J52" s="19">
         <f>L71*B34</f>
         <v>104.08824719790415</v>
       </c>
@@ -1911,7 +1842,7 @@
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L52" s="15">
+      <c r="L52" s="13">
         <f>H71 + I71/J71</f>
         <v>3.9088110924995347E-2</v>
       </c>
@@ -1921,19 +1852,19 @@
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
-        <v>57</v>
+      <c r="A53" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B53" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C53" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D53" t="s">
-        <v>22</v>
-      </c>
-      <c r="J53" s="21">
+        <v>14</v>
+      </c>
+      <c r="J53" s="19">
         <f>L72*N53*B34</f>
         <v>223.87212597208145</v>
       </c>
@@ -1941,7 +1872,7 @@
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L53" s="15">
+      <c r="L53" s="13">
         <v>0.01</v>
       </c>
       <c r="M53" t="str">
@@ -1965,23 +1896,23 @@
         <v>1/h</v>
       </c>
       <c r="T53" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A54" s="8" t="s">
-        <v>55</v>
+      <c r="A54" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="B54" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C54" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D54" t="s">
-        <v>22</v>
-      </c>
-      <c r="J54" s="21">
+        <v>14</v>
+      </c>
+      <c r="J54" s="19">
         <f>L73*B34</f>
         <v>548.78374889246641</v>
       </c>
@@ -1989,7 +1920,7 @@
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L54" s="15">
+      <c r="L54" s="13">
         <f>H73 + I73/J73</f>
         <v>2.5047272727272724E-2</v>
       </c>
@@ -1999,22 +1930,22 @@
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A55" s="8" t="s">
-        <v>55</v>
+      <c r="A55" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="B55" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C55" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D55" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G55" t="s">
-        <v>52</v>
-      </c>
-      <c r="J55" s="21">
+        <v>44</v>
+      </c>
+      <c r="J55" s="19">
         <f>L74*B34</f>
         <v>181.49756560590552</v>
       </c>
@@ -2022,29 +1953,29 @@
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L55" s="15"/>
+      <c r="L55" s="13"/>
       <c r="M55" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A56" s="8" t="s">
-        <v>94</v>
+      <c r="A56" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="B56" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C56" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D56" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E56" t="s">
-        <v>38</v>
-      </c>
-      <c r="J56" s="21">
+        <v>30</v>
+      </c>
+      <c r="J56" s="19">
         <f>L75*B34</f>
         <v>43.92</v>
       </c>
@@ -2052,7 +1983,7 @@
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L56" s="15">
+      <c r="L56" s="13">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="M56" t="str">
@@ -2064,19 +1995,19 @@
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
-        <v>95</v>
+      <c r="A57" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="B57" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C57" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D57" t="s">
-        <v>38</v>
-      </c>
-      <c r="J57" s="21">
+        <v>30</v>
+      </c>
+      <c r="J57" s="19">
         <f>L76*B34</f>
         <v>0.140544</v>
       </c>
@@ -2084,7 +2015,7 @@
         <f>B42 &amp; "/time range/" &amp; B41 &amp; B40</f>
         <v>$/time range/kWh</v>
       </c>
-      <c r="L57" s="15"/>
+      <c r="L57" s="13"/>
       <c r="M57" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
@@ -2094,22 +2025,22 @@
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A58" s="8" t="s">
-        <v>94</v>
+      <c r="A58" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="B58" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C58" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D58" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E58" t="s">
-        <v>22</v>
-      </c>
-      <c r="J58" s="21">
+        <v>14</v>
+      </c>
+      <c r="J58" s="19">
         <f>L77*B34</f>
         <v>17.568000000000001</v>
       </c>
@@ -2117,7 +2048,7 @@
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L58" s="15"/>
+      <c r="L58" s="13"/>
       <c r="M58" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
@@ -2128,357 +2059,357 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A64" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B64" s="15"/>
-      <c r="C64" s="15"/>
-      <c r="L64" s="9"/>
-      <c r="M64" s="9"/>
+      <c r="A64" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
+      <c r="L64" s="7"/>
+      <c r="M64" s="7"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>88</v>
-      </c>
-      <c r="L65" s="9"/>
-      <c r="M65" s="9"/>
+        <v>80</v>
+      </c>
+      <c r="L65" s="7"/>
+      <c r="M65" s="7"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A67" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B67" s="11"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="11"/>
-      <c r="J67" s="11"/>
-      <c r="K67" s="11"/>
+      <c r="A67" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="9"/>
+      <c r="K67" s="9"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A68" s="12"/>
-      <c r="B68" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C68" s="14">
+      <c r="A68" s="10"/>
+      <c r="B68" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C68" s="12">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D68" s="16"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
-      <c r="H68" s="16"/>
-      <c r="I68" s="16"/>
-      <c r="J68" s="16"/>
-      <c r="K68" s="16"/>
-      <c r="L68" s="16"/>
-      <c r="M68" s="16"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+      <c r="K68" s="14"/>
+      <c r="L68" s="14"/>
+      <c r="M68" s="14"/>
     </row>
     <row r="69" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
-      <c r="B69" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C69" s="19" t="str">
+      <c r="B69" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C69" s="17" t="str">
         <f xml:space="preserve"> "Overnight cost [" &amp; B42 &amp; "/" &amp; B41 &amp; "]"</f>
         <v>Overnight cost [$/kW]</v>
       </c>
-      <c r="D69" s="13" t="str">
+      <c r="D69" s="11" t="str">
         <f xml:space="preserve"> "Fixed O&amp;M cost ["  &amp; B42 &amp; "/" &amp; B41 &amp; "year]"</f>
         <v>Fixed O&amp;M cost [$/kWyear]</v>
       </c>
-      <c r="E69" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F69" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="G69" s="17" t="str">
+      <c r="E69" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F69" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G69" s="15" t="str">
         <f xml:space="preserve"> "Annual fixed costs [" &amp;B42 &amp; "/year]"</f>
         <v>Annual fixed costs [$/year]</v>
       </c>
-      <c r="H69" s="13" t="str">
+      <c r="H69" s="11" t="str">
         <f xml:space="preserve"> "Variable O&amp;M [" &amp; B42 &amp; "/" &amp; B41 &amp; B40 &amp; "]"</f>
         <v>Variable O&amp;M [$/kWh]</v>
       </c>
-      <c r="I69" s="13" t="str">
+      <c r="I69" s="11" t="str">
         <f xml:space="preserve"> "Fuel cost [" &amp; B42 &amp; "/" &amp; B41 &amp; B40 &amp; "]"</f>
         <v>Fuel cost [$/kWh]</v>
       </c>
-      <c r="J69" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="K69" s="19"/>
-      <c r="L69" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="M69" s="13"/>
+      <c r="J69" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="K69" s="17"/>
+      <c r="L69" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M69" s="11"/>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B70" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C70" s="20">
+      <c r="B70" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C70" s="18">
         <v>1851</v>
       </c>
-      <c r="D70" s="14">
+      <c r="D70" s="12">
         <v>22.02</v>
       </c>
-      <c r="E70" s="14">
+      <c r="E70" s="12">
         <f>C68*(1+C68)^F70/((1+C68)^F70-1)</f>
         <v>8.0586403511111196E-2</v>
       </c>
-      <c r="F70" s="14">
+      <c r="F70" s="12">
         <v>30</v>
       </c>
-      <c r="G70" s="18">
+      <c r="G70" s="16">
         <f>C70*E70+D70</f>
         <v>171.18543289906683</v>
       </c>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="14"/>
-      <c r="K70" s="20"/>
-      <c r="L70" s="14">
+      <c r="H70" s="12"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="12"/>
+      <c r="K70" s="18"/>
+      <c r="L70" s="12">
         <f>G70/8760</f>
         <v>1.954171608436836E-2</v>
       </c>
-      <c r="M70" s="14" t="str">
+      <c r="M70" s="12" t="str">
         <f>B42&amp;"/"&amp;B40&amp;"/"&amp;B41</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B71" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C71" s="20">
+      <c r="B71" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C71" s="18">
         <v>982</v>
       </c>
-      <c r="D71" s="14">
+      <c r="D71" s="12">
         <v>11.11</v>
       </c>
-      <c r="E71" s="14">
+      <c r="E71" s="12">
         <f>C68*(1+C68)^F71/((1+C68)^F71-1)</f>
         <v>9.4392925743255696E-2</v>
       </c>
-      <c r="F71" s="14">
+      <c r="F71" s="12">
         <v>20</v>
       </c>
-      <c r="G71" s="18">
+      <c r="G71" s="16">
         <f>C71*E71+D71</f>
         <v>103.80385307987709</v>
       </c>
-      <c r="H71" s="14">
+      <c r="H71" s="12">
         <v>3.5400000000000002E-3</v>
       </c>
-      <c r="I71" s="14">
+      <c r="I71" s="12">
         <v>1.9099999999999999E-2</v>
       </c>
-      <c r="J71" s="14">
+      <c r="J71" s="12">
         <v>0.5373</v>
       </c>
-      <c r="K71" s="20"/>
-      <c r="L71" s="14">
+      <c r="K71" s="18"/>
+      <c r="L71" s="12">
         <f>G71/8760</f>
         <v>1.1849754917794188E-2</v>
       </c>
-      <c r="M71" s="14" t="str">
+      <c r="M71" s="12" t="str">
         <f>B42&amp;"/"&amp;B40&amp;"/"&amp;B41</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B72" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C72" s="20">
+      <c r="B72" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C72" s="18">
         <v>261</v>
       </c>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14">
+      <c r="D72" s="12"/>
+      <c r="E72" s="12">
         <f>C68*(1+C68)^F72/((1+C68)^F72-1)</f>
         <v>0.14237750272736471</v>
       </c>
-      <c r="F72" s="14">
+      <c r="F72" s="12">
         <v>10</v>
       </c>
-      <c r="G72" s="18">
+      <c r="G72" s="16">
         <f>C72*E72+D72</f>
         <v>37.160528211842191</v>
       </c>
-      <c r="H72" s="14"/>
-      <c r="I72" s="14"/>
-      <c r="J72" s="14"/>
-      <c r="K72" s="20"/>
-      <c r="L72" s="14">
+      <c r="H72" s="12"/>
+      <c r="I72" s="12"/>
+      <c r="J72" s="12"/>
+      <c r="K72" s="18"/>
+      <c r="L72" s="12">
         <f>G72/8760</f>
         <v>4.2420694305755928E-3</v>
       </c>
-      <c r="M72" s="14" t="str">
+      <c r="M72" s="12" t="str">
         <f>B42&amp;"/"&amp;B40&amp;"/"&amp;B41</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B73" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C73" s="20">
+      <c r="B73" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73" s="18">
         <v>5946</v>
       </c>
-      <c r="D73" s="14">
+      <c r="D73" s="12">
         <v>101.28</v>
       </c>
-      <c r="E73" s="14">
+      <c r="E73" s="12">
         <f>C68*(1+C68)^F73/((1+C68)^F73-1)</f>
         <v>7.5009138873610326E-2</v>
       </c>
-      <c r="F73" s="14">
+      <c r="F73" s="12">
         <v>40</v>
       </c>
-      <c r="G73" s="18">
+      <c r="G73" s="16">
         <f>C73*E73+D73</f>
         <v>547.28433974248696</v>
       </c>
-      <c r="H73" s="14">
+      <c r="H73" s="12">
         <v>2.32E-3</v>
       </c>
-      <c r="I73" s="14">
+      <c r="I73" s="12">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="J73" s="14">
+      <c r="J73" s="12">
         <v>0.33</v>
       </c>
-      <c r="K73" s="20"/>
-      <c r="L73" s="14">
+      <c r="K73" s="18"/>
+      <c r="L73" s="12">
         <f>G73/8760</f>
         <v>6.2475381249142349E-2</v>
       </c>
-      <c r="M73" s="14" t="str">
+      <c r="M73" s="12" t="str">
         <f>B42&amp;"/"&amp;B40&amp;"/"&amp;B41</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B74" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C74" s="20">
+      <c r="B74" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C74" s="18">
         <v>1657</v>
       </c>
-      <c r="D74" s="14">
+      <c r="D74" s="12">
         <v>47.47</v>
       </c>
-      <c r="E74" s="14">
+      <c r="E74" s="12">
         <f>C68*(1+C68)^F74/((1+C68)^F74-1)</f>
         <v>8.0586403511111196E-2</v>
       </c>
-      <c r="F74" s="14">
+      <c r="F74" s="12">
         <v>30</v>
       </c>
-      <c r="G74" s="18">
+      <c r="G74" s="16">
         <f>C74*E74+D74</f>
         <v>181.00167061791126</v>
       </c>
-      <c r="H74" s="14"/>
-      <c r="I74" s="14"/>
-      <c r="J74" s="14"/>
-      <c r="K74" s="20"/>
-      <c r="L74" s="14">
+      <c r="H74" s="12"/>
+      <c r="I74" s="12"/>
+      <c r="J74" s="12"/>
+      <c r="K74" s="18"/>
+      <c r="L74" s="12">
         <f>G74/8760</f>
         <v>2.0662291166428225E-2</v>
       </c>
-      <c r="M74" s="14" t="str">
+      <c r="M74" s="12" t="str">
         <f>B42&amp;"/"&amp;B40&amp;"/"&amp;B41</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B75" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C75" s="20"/>
-      <c r="D75" s="14"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="14"/>
-      <c r="G75" s="18"/>
-      <c r="H75" s="14"/>
-      <c r="I75" s="14"/>
-      <c r="J75" s="18"/>
-      <c r="K75" s="14"/>
-      <c r="L75" s="14">
+      <c r="B75" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C75" s="18"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="16"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="12"/>
+      <c r="J75" s="16"/>
+      <c r="K75" s="12"/>
+      <c r="L75" s="12">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="M75" s="14" t="str">
+      <c r="M75" s="12" t="str">
         <f>B42&amp;"/"&amp;B40&amp;"/"&amp;B41</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B76" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C76" s="20"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="18"/>
-      <c r="H76" s="14"/>
-      <c r="I76" s="14"/>
-      <c r="J76" s="18"/>
-      <c r="K76" s="14"/>
-      <c r="L76" s="14">
+      <c r="B76" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C76" s="18"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="16"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="16"/>
+      <c r="K76" s="12"/>
+      <c r="L76" s="12">
         <v>1.5999999999999999E-5</v>
       </c>
-      <c r="M76" s="14" t="str">
+      <c r="M76" s="12" t="str">
         <f>B42&amp;"/"&amp;B40&amp;"/"&amp;B41</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B77" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C77" s="20"/>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="18"/>
-      <c r="H77" s="14"/>
-      <c r="I77" s="14"/>
-      <c r="J77" s="18"/>
-      <c r="K77" s="14"/>
-      <c r="L77" s="14">
+      <c r="B77" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C77" s="18"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="16"/>
+      <c r="H77" s="12"/>
+      <c r="I77" s="12"/>
+      <c r="J77" s="16"/>
+      <c r="K77" s="12"/>
+      <c r="L77" s="12">
         <v>2E-3</v>
       </c>
-      <c r="M77" s="14" t="str">
+      <c r="M77" s="12" t="str">
         <f>B42&amp;"/"&amp;B40&amp;"/"&amp;B41</f>
         <v>$/h/kW</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed scaling, cylic E, op.cost unit
</commit_message>
<xml_diff>
--- a/test/test_case.xlsx
+++ b/test/test_case.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/CLab/clab_pypsa/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/Library/Group Containers/G69SCX94XU.duck/Library/Application Support/duck/Volumes.noindex/DPB-DGE Data Transfer Node/nobackup/scratch/awongel/clab_pypsa/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8C1AF6-34A8-D047-B7E1-6391DB489272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16FC805-3471-584E-AE82-A1DBAE002B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="880" windowWidth="28500" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1282,8 +1282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2020,6 +2020,9 @@
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
       </c>
+      <c r="O57" t="b">
+        <v>1</v>
+      </c>
       <c r="R57" s="1">
         <v>3.9999999999999998E-6</v>
       </c>

</xml_diff>

<commit_message>
Allow time series for any attribute
</commit_message>
<xml_diff>
--- a/test/test_case.xlsx
+++ b/test/test_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/Library/Group Containers/G69SCX94XU.duck/Library/Application Support/duck/Volumes.noindex/DPB-DGE Data Transfer Node/nobackup/scratch/awongel/clab_pypsa/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/Library/Group Containers/G69SCX94XU.duck/Library/Application Support/duck/Volumes.noindex/DPB-DGE Data Transfer Node.localized/nobackup/scratch/awongel/clab_borehole_th_storage/table_pypsa/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16FC805-3471-584E-AE82-A1DBAE002B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99C8128-79BD-E849-9A7C-33E766523264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="880" windowWidth="28500" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28500" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input_intermodel_one_node_" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="103">
   <si>
     <t>Note that demand has no decisions.</t>
   </si>
@@ -59,9 +59,6 @@
     <t>numerics_scaling</t>
   </si>
   <si>
-    <t>normalization</t>
-  </si>
-  <si>
     <t>efficiency</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>bus</t>
   </si>
   <si>
-    <t>p_nom</t>
-  </si>
-  <si>
     <t>capital_cost</t>
   </si>
   <si>
@@ -329,9 +323,6 @@
     <t>https://raw.githubusercontent.com/PyPSA/technology-data/master/outputs/costs_2020.csv</t>
   </si>
   <si>
-    <t>p_min_pu</t>
-  </si>
-  <si>
     <t>Note: p_min_pu allow bidirectionality of link</t>
   </si>
   <si>
@@ -345,6 +336,12 @@
   </si>
   <si>
     <t>test/</t>
+  </si>
+  <si>
+    <t>p_set</t>
+  </si>
+  <si>
+    <t>p_max_pu</t>
   </si>
 </sst>
 </file>
@@ -984,9 +981,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1024,7 +1021,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1130,7 +1127,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1272,7 +1269,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1280,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T78"/>
+  <dimension ref="A1:R78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1307,7 +1304,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1325,7 +1322,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1363,7 +1360,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1391,10 +1388,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1403,10 +1400,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1415,10 +1412,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1445,10 +1442,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1457,10 +1454,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1469,10 +1466,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1481,10 +1478,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1493,10 +1490,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1505,10 +1502,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1517,10 +1514,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1534,18 +1531,18 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1553,7 +1550,7 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1561,41 +1558,41 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C31" s="6"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1604,19 +1601,19 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B33" s="19">
         <f>(B31-B30)*24/B32</f>
         <v>8784</v>
       </c>
       <c r="C33" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B34" s="19">
         <f>B33*B32</f>
@@ -1629,23 +1626,23 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C36" s="4"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
@@ -1657,7 +1654,7 @@
       </c>
       <c r="C38" s="1"/>
       <c r="D38" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
@@ -1666,28 +1663,28 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C42" s="1"/>
     </row>
@@ -1695,389 +1692,383 @@
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="F43" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I44" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D45" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H45" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="O45" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D49" s="2" t="s">
+      <c r="E49" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F49" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="G49" s="2" t="s">
+      <c r="J49" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H49" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N49" s="2" t="s">
+      <c r="B50" t="s">
         <v>18</v>
       </c>
-      <c r="O49" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q49" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="R49" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B50" t="s">
-        <v>20</v>
-      </c>
       <c r="C50" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G50" t="s">
-        <v>42</v>
-      </c>
-      <c r="J50" s="19">
+        <v>40</v>
+      </c>
+      <c r="H50" s="19">
         <f>L70*B34</f>
         <v>171.65443408509168</v>
       </c>
-      <c r="K50" t="str">
+      <c r="I50" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L50" s="13"/>
-      <c r="M50" t="str">
+      <c r="J50" s="13"/>
+      <c r="K50" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D51" t="s">
-        <v>14</v>
-      </c>
-      <c r="G51" t="s">
-        <v>43</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F51" t="s">
+        <v>41</v>
+      </c>
+      <c r="H51" s="13"/>
       <c r="J51" s="13"/>
-      <c r="L51" s="13"/>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B52" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C52" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D52" t="s">
-        <v>14</v>
-      </c>
-      <c r="J52" s="19">
+        <v>13</v>
+      </c>
+      <c r="H52" s="19">
         <f>L71*B34</f>
         <v>104.08824719790415</v>
       </c>
-      <c r="K52" t="str">
+      <c r="I52" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L52" s="13">
+      <c r="J52" s="13">
         <f>H71 + I71/J71</f>
         <v>3.9088110924995347E-2</v>
       </c>
-      <c r="M52" t="str">
+      <c r="K52" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B53" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C53" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D53" t="s">
-        <v>14</v>
-      </c>
-      <c r="J53" s="19">
-        <f>L72*N53*B34</f>
+        <v>13</v>
+      </c>
+      <c r="H53" s="19">
+        <f>L72*L53*B34</f>
         <v>223.87212597208145</v>
       </c>
-      <c r="K53" t="str">
+      <c r="I53" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L53" s="13">
+      <c r="J53" s="13">
         <v>0.01</v>
       </c>
-      <c r="M53" t="str">
+      <c r="K53" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
       </c>
+      <c r="L53">
+        <v>6.008</v>
+      </c>
+      <c r="M53" t="b">
+        <v>1</v>
+      </c>
       <c r="N53">
-        <v>6.008</v>
-      </c>
-      <c r="O53" t="b">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="P53">
-        <v>0.9</v>
-      </c>
-      <c r="R53">
         <v>1.1400000000000001E-6</v>
       </c>
-      <c r="S53" t="str">
+      <c r="Q53" t="str">
         <f xml:space="preserve"> 1 &amp; "/" &amp; B40</f>
         <v>1/h</v>
       </c>
-      <c r="T53" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B54" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C54" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D54" t="s">
-        <v>14</v>
-      </c>
-      <c r="J54" s="19">
+        <v>13</v>
+      </c>
+      <c r="H54" s="19">
         <f>L73*B34</f>
         <v>548.78374889246641</v>
       </c>
-      <c r="K54" t="str">
+      <c r="I54" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L54" s="13">
+      <c r="J54" s="13">
         <f>H73 + I73/J73</f>
         <v>2.5047272727272724E-2</v>
       </c>
-      <c r="M54" t="str">
+      <c r="K54" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B55" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C55" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G55" t="s">
-        <v>44</v>
-      </c>
-      <c r="J55" s="19">
+        <v>42</v>
+      </c>
+      <c r="H55" s="19">
         <f>L74*B34</f>
         <v>181.49756560590552</v>
       </c>
-      <c r="K55" t="str">
+      <c r="I55" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L55" s="13"/>
-      <c r="M55" t="str">
+      <c r="J55" s="13"/>
+      <c r="K55" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B56" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" t="s">
         <v>28</v>
       </c>
-      <c r="C56" t="s">
-        <v>28</v>
-      </c>
-      <c r="D56" t="s">
-        <v>14</v>
-      </c>
-      <c r="E56" t="s">
-        <v>30</v>
-      </c>
-      <c r="J56" s="19">
+      <c r="H56" s="19">
         <f>L75*B34</f>
         <v>43.92</v>
       </c>
-      <c r="K56" t="str">
+      <c r="I56" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L56" s="13">
+      <c r="J56" s="13">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M56" t="str">
+      <c r="K56" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
       </c>
-      <c r="P56">
+      <c r="N56">
         <v>0.7</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B57" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C57" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D57" t="s">
-        <v>30</v>
-      </c>
-      <c r="J57" s="19">
+        <v>28</v>
+      </c>
+      <c r="H57" s="19">
         <f>L76*B34</f>
         <v>0.140544</v>
       </c>
-      <c r="K57" t="str">
+      <c r="I57" t="str">
         <f>B42 &amp; "/time range/" &amp; B41 &amp; B40</f>
         <v>$/time range/kWh</v>
       </c>
-      <c r="L57" s="13"/>
-      <c r="M57" t="str">
+      <c r="J57" s="13"/>
+      <c r="K57" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
       </c>
-      <c r="O57" t="b">
+      <c r="M57" t="b">
         <v>1</v>
       </c>
-      <c r="R57" s="1">
+      <c r="P57" s="1">
         <v>3.9999999999999998E-6</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B58" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C58" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D58" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E58" t="s">
-        <v>14</v>
-      </c>
-      <c r="J58" s="19">
+        <v>13</v>
+      </c>
+      <c r="H58" s="19">
         <f>L77*B34</f>
         <v>17.568000000000001</v>
       </c>
-      <c r="K58" t="str">
+      <c r="I58" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="L58" s="13"/>
-      <c r="M58" t="str">
+      <c r="J58" s="13"/>
+      <c r="K58" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/kWh</v>
       </c>
-      <c r="P58">
+      <c r="N58">
         <v>0.5</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
@@ -2086,14 +2077,14 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L65" s="7"/>
       <c r="M65" s="7"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
@@ -2111,7 +2102,7 @@
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="10"/>
       <c r="B68" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C68" s="12">
         <v>7.0000000000000007E-2</v>
@@ -2130,7 +2121,7 @@
     <row r="69" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C69" s="17" t="str">
         <f xml:space="preserve"> "Overnight cost [" &amp; B42 &amp; "/" &amp; B41 &amp; "]"</f>
@@ -2141,10 +2132,10 @@
         <v>Fixed O&amp;M cost [$/kWyear]</v>
       </c>
       <c r="E69" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F69" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="F69" s="11" t="s">
-        <v>78</v>
       </c>
       <c r="G69" s="15" t="str">
         <f xml:space="preserve"> "Annual fixed costs [" &amp;B42 &amp; "/year]"</f>
@@ -2159,17 +2150,17 @@
         <v>Fuel cost [$/kWh]</v>
       </c>
       <c r="J69" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K69" s="17"/>
       <c r="L69" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M69" s="11"/>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B70" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C70" s="18">
         <v>1851</v>
@@ -2203,7 +2194,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B71" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C71" s="18">
         <v>982</v>
@@ -2243,7 +2234,7 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B72" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C72" s="18">
         <v>261</v>
@@ -2275,7 +2266,7 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B73" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C73" s="18">
         <v>5946</v>
@@ -2315,7 +2306,7 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B74" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C74" s="18">
         <v>1657</v>
@@ -2349,7 +2340,7 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B75" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C75" s="18"/>
       <c r="D75" s="12"/>
@@ -2370,7 +2361,7 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B76" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C76" s="18"/>
       <c r="D76" s="12"/>
@@ -2391,7 +2382,7 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B77" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C77" s="18"/>
       <c r="D77" s="12"/>
@@ -2412,7 +2403,7 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix extra hour bug
</commit_message>
<xml_diff>
--- a/test/test_case.xlsx
+++ b/test/test_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/Library/Group Containers/G69SCX94XU.duck/Library/Application Support/duck/Volumes.noindex/DPB-DGE Data Transfer Node.localized/nobackup/scratch/awongel/clab_borehole_th_storage/table_pypsa/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/m_/v6c97p3x1mg6bmvchddj43dc0000gn/T/fz3temp-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99C8128-79BD-E849-9A7C-33E766523264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A6F08D-A76A-164F-976A-DBB710F85459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28500" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="760" windowWidth="28500" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input_intermodel_one_node_" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="104">
   <si>
     <t>Note that demand has no decisions.</t>
   </si>
@@ -281,9 +281,6 @@
     <t>Note: This is a test case, the costs aren't meant to be very realistic but provide reproducibility in tests</t>
   </si>
   <si>
-    <t>2017-01-01 0:00:00</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -342,6 +339,12 @@
   </si>
   <si>
     <t>p_max_pu</t>
+  </si>
+  <si>
+    <t>Note: End datetime is defined as the last hour that is included in the time series</t>
+  </si>
+  <si>
+    <t>2016-12-31 23:00:00</t>
   </si>
 </sst>
 </file>
@@ -1279,8 +1282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1322,7 +1325,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1534,15 +1537,15 @@
         <v>35</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" s="21" t="s">
         <v>94</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1558,7 +1561,7 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1566,7 +1569,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1574,7 +1577,7 @@
         <v>32</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" t="s">
@@ -1586,9 +1589,12 @@
         <v>33</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="C31" s="6"/>
+      <c r="D31" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -1601,23 +1607,23 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33" s="19">
-        <f>(B31-B30)*24/B32</f>
-        <v>8784</v>
+        <f>(B31-B30)*24/B32+1</f>
+        <v>8784.0000000000582</v>
       </c>
       <c r="C33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B34" s="19">
         <f>B33*B32</f>
-        <v>8784</v>
+        <v>8784.0000000000582</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
@@ -1626,10 +1632,10 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="22" t="s">
         <v>97</v>
-      </c>
-      <c r="B36" s="22" t="s">
-        <v>98</v>
       </c>
       <c r="C36" s="4"/>
     </row>
@@ -1672,7 +1678,7 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>70</v>
@@ -1692,7 +1698,7 @@
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="F43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -1716,7 +1722,7 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:18" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
@@ -1736,10 +1742,10 @@
         <v>27</v>
       </c>
       <c r="F49" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G49" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>14</v>
@@ -1781,7 +1787,7 @@
       </c>
       <c r="H50" s="19">
         <f>L70*B34</f>
-        <v>171.65443408509168</v>
+        <v>171.65443408509282</v>
       </c>
       <c r="I50" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
@@ -1827,7 +1833,7 @@
       </c>
       <c r="H52" s="19">
         <f>L71*B34</f>
-        <v>104.08824719790415</v>
+        <v>104.08824719790483</v>
       </c>
       <c r="I52" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
@@ -1857,7 +1863,7 @@
       </c>
       <c r="H53" s="19">
         <f>L72*L53*B34</f>
-        <v>223.87212597208145</v>
+        <v>223.87212597208293</v>
       </c>
       <c r="I53" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
@@ -1905,7 +1911,7 @@
       </c>
       <c r="H54" s="19">
         <f>L73*B34</f>
-        <v>548.78374889246641</v>
+        <v>548.78374889247004</v>
       </c>
       <c r="I54" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
@@ -1938,7 +1944,7 @@
       </c>
       <c r="H55" s="19">
         <f>L74*B34</f>
-        <v>181.49756560590552</v>
+        <v>181.49756560590671</v>
       </c>
       <c r="I55" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
@@ -1952,7 +1958,7 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B56" t="s">
         <v>26</v>
@@ -1968,7 +1974,7 @@
       </c>
       <c r="H56" s="19">
         <f>L75*B34</f>
-        <v>43.92</v>
+        <v>43.920000000000293</v>
       </c>
       <c r="I56" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
@@ -1987,7 +1993,7 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B57" t="s">
         <v>29</v>
@@ -2000,7 +2006,7 @@
       </c>
       <c r="H57" s="19">
         <f>L76*B34</f>
-        <v>0.140544</v>
+        <v>0.14054400000000092</v>
       </c>
       <c r="I57" t="str">
         <f>B42 &amp; "/time range/" &amp; B41 &amp; B40</f>
@@ -2020,7 +2026,7 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B58" t="s">
         <v>30</v>
@@ -2036,7 +2042,7 @@
       </c>
       <c r="H58" s="19">
         <f>L77*B34</f>
-        <v>17.568000000000001</v>
+        <v>17.568000000000115</v>
       </c>
       <c r="I58" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
@@ -2053,7 +2059,7 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>